<commit_message>
CPPD internal analysis worksheet - total != sum of other rows, needs clarification
</commit_message>
<xml_diff>
--- a/Assoc. of WA Cities Signatories/College Place - closed/Data/3 year comparison.xlsx
+++ b/Assoc. of WA Cities Signatories/College Place - closed/Data/3 year comparison.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="V:\PD Shared\Command\Pursuits\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marti\Documents\GitHub\wa-pursuit-pdr-data\Assoc. of WA Cities Signatories\College Place - closed\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D12FD75-06A5-43D1-9EB5-EFFC4866DCB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2710925-7913-4EBA-8041-DB20687F0A74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Authorized</t>
   </si>
@@ -44,12 +44,15 @@
   <si>
     <t xml:space="preserve">Number of pursuits </t>
   </si>
+  <si>
+    <t>NOTE:  The total does NOT equal the sum of Authorized + Unauthorized</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -61,6 +64,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -125,7 +135,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -143,6 +153,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2498,10 +2509,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A5:J9"/>
+  <dimension ref="A5:L9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:J9"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2509,7 +2520,7 @@
     <col min="2" max="2" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -2539,7 +2550,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>5</v>
       </c>
@@ -2568,8 +2579,11 @@
       <c r="J6" s="3">
         <v>37</v>
       </c>
+      <c r="L6" s="11" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
@@ -2599,7 +2613,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>1</v>
       </c>
@@ -2629,7 +2643,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>2</v>
       </c>

</xml_diff>